<commit_message>
changed the fields to text.
</commit_message>
<xml_diff>
--- a/unittests/test_cases/sample_test.xlsx
+++ b/unittests/test_cases/sample_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\FCM_Projects\FCM_Python\FCM_BCI\PyFcmBci\unittests\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75926A5-5F62-426B-A094-A131B905B824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB054413-42BC-420C-9295-4310D4C85338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34620" yWindow="2280" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expert_1" sheetId="1" r:id="rId1"/>
@@ -50,28 +50,28 @@
     <t>C4</t>
   </si>
   <si>
-    <t>"M"</t>
-  </si>
-  <si>
-    <t>"VH"</t>
-  </si>
-  <si>
-    <t>"H"</t>
-  </si>
-  <si>
-    <t>"L"</t>
-  </si>
-  <si>
-    <t>"VL"</t>
-  </si>
-  <si>
-    <t>"-M"</t>
-  </si>
-  <si>
-    <t>"-H"</t>
-  </si>
-  <si>
-    <t>"-VH"</t>
+    <t>VH</t>
+  </si>
+  <si>
+    <t>-VH</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>-H</t>
+  </si>
+  <si>
+    <t>VL</t>
+  </si>
+  <si>
+    <t>-M</t>
   </si>
 </sst>
 </file>
@@ -115,10 +115,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,61 +403,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="232" zoomScaleNormal="232" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="232" zoomScaleNormal="232" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -467,66 +480,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92C0005-4004-4F2D-A51F-E30CE0F2B5F6}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="237" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -538,63 +579,78 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -606,61 +662,79 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1822E663-592E-426B-AEB5-23382CDCF484}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="246" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -669,115 +743,153 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32998B3A-F618-40E0-AF94-547EE5EE1BD2}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView zoomScale="247" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76592AC3-AD17-4C06-867D-3A73A4803FAB}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="247" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="225" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76592AC3-AD17-4C06-867D-3A73A4803FAB}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView zoomScale="225" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>